<commit_message>
fix: add two drinks
</commit_message>
<xml_diff>
--- a/bev_name.xlsx
+++ b/bev_name.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64085F34-2D58-40E8-B66A-296E23120064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C460B7A-30EE-4C35-A09C-631BAC706DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="205">
   <si>
     <t>BSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -757,6 +757,14 @@
   </si>
   <si>
     <t>太窄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>康师傅水蜜桃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>康师傅绿茶</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1140,18 +1148,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1179,7 +1187,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1207,7 +1215,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1221,7 +1229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1235,7 +1243,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1249,7 +1257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1263,7 +1271,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1291,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1305,7 +1313,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1333,7 +1341,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1347,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -1361,7 +1369,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -1375,7 +1383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1389,7 +1397,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1417,7 +1425,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1431,7 +1439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1445,7 +1453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -1459,7 +1467,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -1487,7 +1495,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +1509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1515,7 +1523,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1529,7 +1537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1543,7 +1551,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1599,7 +1607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1613,7 +1621,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1627,7 +1635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1641,7 +1649,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1655,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1669,7 +1677,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1683,7 +1691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1711,7 +1719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1725,7 +1733,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1753,7 +1761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -1767,7 +1775,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -1795,7 +1803,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1809,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -1823,7 +1831,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1851,7 +1859,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -1879,7 +1887,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -1893,7 +1901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -1907,7 +1915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -1921,7 +1929,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1935,7 +1943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1949,7 +1957,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -1963,7 +1971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1991,7 +1999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -2005,7 +2013,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -2019,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>99</v>
       </c>
@@ -2033,7 +2041,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>97</v>
       </c>
@@ -2047,7 +2055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -2061,7 +2069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>52</v>
       </c>
@@ -2075,7 +2083,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2111,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2117,7 +2125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -2131,7 +2139,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>40</v>
       </c>
@@ -2145,7 +2153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -2159,7 +2167,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -2173,7 +2181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -2187,7 +2195,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -2201,7 +2209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -2215,7 +2223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2229,7 +2237,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2257,7 +2265,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -2271,7 +2279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -2285,7 +2293,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -2299,7 +2307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -2313,7 +2321,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>21</v>
       </c>
@@ -2327,7 +2335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>54</v>
       </c>
@@ -2341,7 +2349,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -2355,7 +2363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -2369,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>29</v>
       </c>
@@ -2383,7 +2391,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -2397,7 +2405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -2411,7 +2419,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>53</v>
       </c>
@@ -2425,7 +2433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -2439,7 +2447,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2453,7 +2461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>43</v>
       </c>
@@ -2467,7 +2475,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -2481,7 +2489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -2495,7 +2503,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>38</v>
       </c>
@@ -2509,7 +2517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -2521,6 +2529,28 @@
       </c>
       <c r="D98">
         <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B99" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" t="s">
+        <v>201</v>
+      </c>
+      <c r="D99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B100" t="s">
+        <v>117</v>
+      </c>
+      <c r="C100" t="s">
+        <v>201</v>
+      </c>
+      <c r="D100">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2537,16 +2567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2557,7 +2587,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2568,7 +2598,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2576,7 +2606,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -2584,7 +2614,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2622,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2600,7 +2630,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2608,7 +2638,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -2616,7 +2646,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -2624,7 +2654,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2632,7 +2662,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2640,7 +2670,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2648,7 +2678,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2656,7 +2686,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2664,7 +2694,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2672,7 +2702,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2680,7 +2710,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -2688,7 +2718,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -2696,7 +2726,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -2704,7 +2734,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -2712,7 +2742,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2720,7 +2750,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2728,7 +2758,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2736,7 +2766,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2744,7 +2774,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2752,7 +2782,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -2760,7 +2790,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2768,7 +2798,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -2776,7 +2806,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2784,7 +2814,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2792,7 +2822,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2800,7 +2830,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2808,7 +2838,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2816,7 +2846,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -2824,7 +2854,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2832,7 +2862,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2840,7 +2870,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2848,15 +2878,15 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2864,7 +2894,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2872,15 +2902,15 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2888,7 +2918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2896,7 +2926,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2904,7 +2934,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2920,7 +2950,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2928,7 +2958,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -2936,7 +2966,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -2944,7 +2974,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -2952,7 +2982,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -2960,7 +2990,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -2968,7 +2998,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -2976,7 +3006,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -2984,7 +3014,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2992,7 +3022,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -3000,7 +3030,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -3008,7 +3038,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3016,7 +3046,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3024,7 +3054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -3032,7 +3062,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3040,7 +3070,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -3048,7 +3078,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -3056,7 +3086,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -3064,7 +3094,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>99</v>
       </c>
@@ -3072,7 +3102,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -3080,7 +3110,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -3088,7 +3118,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>52</v>
       </c>
@@ -3096,7 +3126,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -3104,7 +3134,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -3112,7 +3142,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -3120,7 +3150,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -3128,7 +3158,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -3136,7 +3166,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -3144,7 +3174,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>45</v>
       </c>
@@ -3152,7 +3182,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -3160,7 +3190,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -3168,7 +3198,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -3176,7 +3206,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -3184,7 +3214,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -3192,7 +3222,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -3200,7 +3230,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -3208,7 +3238,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -3216,7 +3246,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -3224,7 +3254,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -3232,7 +3262,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>54</v>
       </c>
@@ -3248,7 +3278,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -3256,7 +3286,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -3264,7 +3294,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>29</v>
       </c>
@@ -3272,7 +3302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>28</v>
       </c>
@@ -3280,7 +3310,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -3288,7 +3318,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>53</v>
       </c>
@@ -3296,7 +3326,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -3304,7 +3334,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -3315,7 +3345,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>43</v>
       </c>
@@ -3326,7 +3356,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -3334,7 +3364,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -3342,7 +3372,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>38</v>
       </c>
@@ -3353,7 +3383,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>37</v>
       </c>
@@ -3377,7 +3407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>